<commit_message>
Integrate GermanMarket class into city generators. Separate year for timer and CO2 factors #96
</commit_message>
<xml_diff>
--- a/pycity_calc/data/BaseData/CO2/co2_gemis_factors.xlsx
+++ b/pycity_calc/data/BaseData/CO2/co2_gemis_factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pycity_calc\pycity_calc\data\BaseData\CO2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pyCity_calc\pycity_calc\data\BaseData\CO2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Prozess</t>
   </si>
@@ -63,13 +63,22 @@
   </si>
   <si>
     <t>Verdrängungsstrom / feed-in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 (2017) in g/kWh End </t>
+  </si>
+  <si>
+    <t>Quelle 2017</t>
+  </si>
+  <si>
+    <t>https://www.ifeu.de/energie/pdf/ifeu_Endbericht_Weiterentwicklung_PEF.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +96,14 @@
       <sz val="10"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -157,6 +174,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -184,8 +203,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>72455</xdr:rowOff>
     </xdr:to>
@@ -580,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,9 +610,10 @@
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,8 +623,14 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -614,8 +640,14 @@
       <c r="C2" s="5">
         <v>313</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5">
+        <v>310</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -625,8 +657,11 @@
       <c r="C3" s="5">
         <v>241</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -636,8 +671,11 @@
       <c r="C4" s="5">
         <v>261</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -647,8 +685,11 @@
       <c r="C5" s="5">
         <v>427</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="5">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -658,8 +699,11 @@
       <c r="C6" s="5">
         <v>449</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="5">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -669,8 +713,11 @@
       <c r="C7" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -680,8 +727,11 @@
       <c r="C8" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -691,8 +741,11 @@
       <c r="C9" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -702,8 +755,11 @@
       <c r="C10" s="5">
         <v>617</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="5">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -713,8 +769,11 @@
       <c r="C11" s="7">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -724,10 +783,14 @@
       <c r="C12" s="7">
         <v>840</v>
       </c>
+      <c r="D12" s="5">
+        <v>840</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add individual CO2 fed-in factors #446
</commit_message>
<xml_diff>
--- a/pycity_calc/data/BaseData/CO2/co2_gemis_factors.xlsx
+++ b/pycity_calc/data/BaseData/CO2/co2_gemis_factors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pyCity_calc\pycity_calc\data\BaseData\CO2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_lokal\pycharm_workspace\pyCity_calc\pycity_calc\data\BaseData\CO2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9975"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="23720" windowHeight="9980"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Prozess</t>
   </si>
@@ -68,10 +68,19 @@
     <t xml:space="preserve">CO2 (2017) in g/kWh End </t>
   </si>
   <si>
-    <t>Quelle 2017</t>
-  </si>
-  <si>
     <t>https://www.ifeu.de/energie/pdf/ifeu_Endbericht_Weiterentwicklung_PEF.pdf</t>
+  </si>
+  <si>
+    <t>http://www.iwu.de/fileadmin/user_upload/dateien/energie/werkzeuge/kea.pdf</t>
+  </si>
+  <si>
+    <t>Quellen</t>
+  </si>
+  <si>
+    <t>https://www.umweltbundesamt.de/publikationen/co2-minderung-im-stromsektor-durch-den-einsatz</t>
+  </si>
+  <si>
+    <t>https://www.umweltbundesamt.de/sites/default/files/medien/378/publikationen/climate_change_11_2016_co2_minderung_im_stromsektor_durch_den_einsatz_erneuerbarer_energien_0.pdf</t>
   </si>
 </sst>
 </file>
@@ -244,7 +253,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>675337</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>189756</xdr:rowOff>
+      <xdr:rowOff>183406</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -602,18 +611,18 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,10 +636,10 @@
         <v>14</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -647,7 +656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -660,8 +669,11 @@
       <c r="D3" s="5">
         <v>242</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -674,8 +686,11 @@
       <c r="D4" s="5">
         <v>258</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -688,8 +703,11 @@
       <c r="D5" s="5">
         <v>419</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -703,7 +721,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -717,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -731,7 +749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -745,7 +763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -759,7 +777,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -773,18 +791,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="7">
-        <v>840</v>
+        <v>810</v>
       </c>
       <c r="C12" s="7">
-        <v>840</v>
+        <v>810</v>
       </c>
       <c r="D12" s="5">
-        <v>840</v>
+        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -800,7 +818,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -812,7 +830,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>